<commit_message>
-Adição do diagrama de sequencia UC14 - Povoar Territorio Conquistado - Acompanhamento do Projeto
</commit_message>
<xml_diff>
--- a/Gerência de Projetos/War - Acompanhamento de Projeto.xlsx
+++ b/Gerência de Projetos/War - Acompanhamento de Projeto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="EstaPasta_de_trabalho"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15195" windowHeight="8700" tabRatio="744" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15195" windowHeight="8700" tabRatio="744" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="6" r:id="rId1"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="260">
   <si>
     <t>Classificação Padrão de Produtos e Serviços</t>
   </si>
@@ -1419,6 +1419,9 @@
   </si>
   <si>
     <t>Diagrama de colaboração/Sequência</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acompanhamento </t>
   </si>
 </sst>
 </file>
@@ -2323,6 +2326,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2345,12 +2354,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2581,11 +2584,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="78606720"/>
-        <c:axId val="78608256"/>
+        <c:axId val="57401728"/>
+        <c:axId val="57403264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78606720"/>
+        <c:axId val="57401728"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2617,7 +2620,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78608256"/>
+        <c:crossAx val="57403264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2625,7 +2628,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78608256"/>
+        <c:axId val="57403264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2667,7 +2670,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78606720"/>
+        <c:crossAx val="57401728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -2713,7 +2716,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598500000354" footer="0.49212598500000354"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598500000365" footer="0.49212598500000365"/>
     <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2751,7 +2754,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.31531602468610342"/>
-          <c:y val="3.2418952618454205E-2"/>
+          <c:y val="3.2418952618454212E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -2768,9 +2771,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.11261286030066738"/>
-          <c:y val="0.14962593516209644"/>
-          <c:w val="0.65090233253786289"/>
-          <c:h val="0.73815461346633926"/>
+          <c:y val="0.14962593516209646"/>
+          <c:w val="0.650902332537863"/>
+          <c:h val="0.73815461346633948"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2927,11 +2930,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78637696"/>
-        <c:axId val="78140160"/>
+        <c:axId val="57813632"/>
+        <c:axId val="57836288"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="78637696"/>
+        <c:axId val="57813632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2963,7 +2966,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78140160"/>
+        <c:crossAx val="57836288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2971,7 +2974,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="78140160"/>
+        <c:axId val="57836288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3014,7 +3017,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78637696"/>
+        <c:crossAx val="57813632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3037,9 +3040,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.7972972972972977"/>
-          <c:y val="0.46882793017456653"/>
+          <c:y val="0.46882793017456664"/>
           <c:w val="0.17792792792792791"/>
-          <c:h val="0.10972568578553761"/>
+          <c:h val="0.10972568578553765"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -3104,7 +3107,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598500000354" footer="0.49212598500000354"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598500000365" footer="0.49212598500000365"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3641,7 +3644,7 @@
       <c r="I2" s="163"/>
       <c r="J2" s="126">
         <f>Parâmetros!B6</f>
-        <v>40317</v>
+        <v>40319</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="6" customHeight="1" thickTop="1"/>
@@ -3652,16 +3655,16 @@
     </row>
     <row r="5" spans="1:11" ht="6" customHeight="1"/>
     <row r="6" spans="1:11" s="137" customFormat="1" ht="27" customHeight="1">
-      <c r="A6" s="184"/>
-      <c r="B6" s="185"/>
-      <c r="C6" s="185"/>
-      <c r="D6" s="185"/>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185"/>
-      <c r="G6" s="185"/>
-      <c r="H6" s="185"/>
-      <c r="I6" s="185"/>
-      <c r="J6" s="185"/>
+      <c r="A6" s="186"/>
+      <c r="B6" s="187"/>
+      <c r="C6" s="187"/>
+      <c r="D6" s="187"/>
+      <c r="E6" s="187"/>
+      <c r="F6" s="187"/>
+      <c r="G6" s="187"/>
+      <c r="H6" s="187"/>
+      <c r="I6" s="187"/>
+      <c r="J6" s="187"/>
       <c r="K6" s="136"/>
     </row>
     <row r="7" spans="1:11" s="137" customFormat="1" ht="6" customHeight="1">
@@ -3817,7 +3820,7 @@
       <c r="B21" s="105"/>
       <c r="C21" s="92">
         <f>Planejamento!I8</f>
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="K21" s="62"/>
     </row>
@@ -3828,7 +3831,7 @@
       <c r="B22" s="105"/>
       <c r="C22" s="92">
         <f>Planejamento!J8</f>
-        <v>26.5</v>
+        <v>32.5</v>
       </c>
       <c r="K22" s="98"/>
     </row>
@@ -3880,11 +3883,11 @@
       <c r="B26" s="196" t="s">
         <v>207</v>
       </c>
-      <c r="C26" s="188"/>
+      <c r="C26" s="190"/>
       <c r="D26" s="196" t="s">
         <v>211</v>
       </c>
-      <c r="E26" s="188"/>
+      <c r="E26" s="190"/>
       <c r="F26" s="89"/>
       <c r="G26" s="93"/>
       <c r="H26" s="93"/>
@@ -4022,18 +4025,18 @@
       <c r="B41" s="206" t="s">
         <v>223</v>
       </c>
-      <c r="C41" s="186" t="s">
+      <c r="C41" s="188" t="s">
         <v>151</v>
       </c>
-      <c r="D41" s="187"/>
-      <c r="E41" s="187"/>
-      <c r="F41" s="188"/>
-      <c r="G41" s="189" t="s">
+      <c r="D41" s="189"/>
+      <c r="E41" s="189"/>
+      <c r="F41" s="190"/>
+      <c r="G41" s="191" t="s">
         <v>160</v>
       </c>
-      <c r="H41" s="190"/>
-      <c r="I41" s="190"/>
-      <c r="J41" s="191"/>
+      <c r="H41" s="192"/>
+      <c r="I41" s="192"/>
+      <c r="J41" s="193"/>
     </row>
     <row r="42" spans="1:11" ht="24.75" customHeight="1">
       <c r="A42" s="85" t="s">
@@ -4096,15 +4099,15 @@
       </c>
       <c r="H43" s="173">
         <f ca="1">Planejamento!I9</f>
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="I43" s="173">
         <f>Planejamento!J9</f>
-        <v>26.5</v>
+        <v>32.5</v>
       </c>
       <c r="J43" s="173">
         <f>Planejamento!K9</f>
-        <v>51.5</v>
+        <v>57.5</v>
       </c>
       <c r="K43" s="107">
         <f>+D43-C43</f>
@@ -4214,11 +4217,11 @@
         <f t="shared" ref="H49" si="5">+IF(C49&lt;&gt;0,D49/C49,0)</f>
         <v>1.9285714285714286</v>
       </c>
-      <c r="I49" s="192">
+      <c r="I49" s="184">
         <f>IF(H49&lt;&gt;0,C49+(VLOOKUP(A49,'Histórico de Versões'!A5:E72,5)-D49)/H49,"")</f>
         <v>141.03703703703704</v>
       </c>
-      <c r="J49" s="193"/>
+      <c r="J49" s="185"/>
     </row>
     <row r="50" spans="1:10" ht="12">
       <c r="A50" s="142">
@@ -4249,11 +4252,11 @@
         <f t="shared" ref="H50:H55" si="7">+IF(C50&lt;&gt;0,D50/C50,0)</f>
         <v>1.9433962264150944</v>
       </c>
-      <c r="I50" s="192">
+      <c r="I50" s="184">
         <f>IF(H50&lt;&gt;0,C50+(VLOOKUP(A50,'Histórico de Versões'!A6:E73,5)-D50)/H50,"")</f>
         <v>139.96116504854371</v>
       </c>
-      <c r="J50" s="193"/>
+      <c r="J50" s="185"/>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="106"/>
@@ -4276,11 +4279,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I51" s="192" t="str">
+      <c r="I51" s="184" t="str">
         <f>IF(H51&lt;&gt;0,C51+(VLOOKUP(A51,'Histórico de Versões'!A7:E74,5)-D51)/H51,"")</f>
         <v/>
       </c>
-      <c r="J51" s="193"/>
+      <c r="J51" s="185"/>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="106"/>
@@ -4303,11 +4306,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I52" s="192" t="str">
+      <c r="I52" s="184" t="str">
         <f>IF(H52&lt;&gt;0,C52+(VLOOKUP(A52,'Histórico de Versões'!A8:E75,5)-D52)/H52,"")</f>
         <v/>
       </c>
-      <c r="J52" s="193"/>
+      <c r="J52" s="185"/>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="106"/>
@@ -4330,11 +4333,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I53" s="192" t="str">
+      <c r="I53" s="184" t="str">
         <f>IF(H53&lt;&gt;0,C53+(VLOOKUP(A53,'Histórico de Versões'!A9:E76,5)-D53)/H53,"")</f>
         <v/>
       </c>
-      <c r="J53" s="193"/>
+      <c r="J53" s="185"/>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="106"/>
@@ -4357,11 +4360,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I54" s="192" t="str">
+      <c r="I54" s="184" t="str">
         <f>IF(H54&lt;&gt;0,C54+(VLOOKUP(A54,'Histórico de Versões'!A10:E77,5)-D54)/H54,"")</f>
         <v/>
       </c>
-      <c r="J54" s="193"/>
+      <c r="J54" s="185"/>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="106"/>
@@ -4384,11 +4387,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I55" s="192" t="str">
+      <c r="I55" s="184" t="str">
         <f>IF(H55&lt;&gt;0,C55+(VLOOKUP(A55,'Histórico de Versões'!A11:E78,5)-D55)/H55,"")</f>
         <v/>
       </c>
-      <c r="J55" s="193"/>
+      <c r="J55" s="185"/>
     </row>
     <row r="56" spans="1:10">
       <c r="B56" s="90"/>
@@ -4403,6 +4406,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="I53:J53"/>
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="C41:F41"/>
@@ -4419,7 +4423,6 @@
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="I51:J51"/>
     <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I53:J53"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.59055118110236227" right="0.51181102362204722" top="0.59055118110236227" bottom="0.59055118110236227" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -4437,10 +4440,10 @@
   </sheetPr>
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A137" sqref="A137"/>
-      <selection pane="topRight" activeCell="A31" sqref="A31"/>
+      <selection pane="topRight" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="2"/>
@@ -4503,7 +4506,7 @@
       <c r="S2" s="146"/>
       <c r="T2" s="95" t="str">
         <f>CONCATENATE("Data Base: ",TEXT(Parâmetros!$B$6,"dd/mm/aaaa"))</f>
-        <v>Data Base: 19/05/2010</v>
+        <v>Data Base: 21/05/2010</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="20.25" customHeight="1" thickTop="1">
@@ -4514,7 +4517,7 @@
       <c r="A5" s="72"/>
       <c r="B5" s="170"/>
       <c r="C5" s="178"/>
-      <c r="D5" s="186" t="s">
+      <c r="D5" s="188" t="s">
         <v>151</v>
       </c>
       <c r="E5" s="208"/>
@@ -4632,19 +4635,19 @@
       </c>
       <c r="I8" s="149">
         <f>SUMIF($B9:$B42,"&gt;0",I9:I42)</f>
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="J8" s="149">
         <f>SUMIF($B9:$B42,"&gt;0",J9:J42)</f>
-        <v>26.5</v>
+        <v>32.5</v>
       </c>
       <c r="K8" s="149">
         <f>SUMIF($B9:$B42,"&gt;0",K9:K42)</f>
-        <v>51.5</v>
+        <v>57.5</v>
       </c>
       <c r="L8" s="150">
         <f>+K8-I8</f>
-        <v>-190.5</v>
+        <v>-214.5</v>
       </c>
       <c r="M8" s="149">
         <f>+K8-J8</f>
@@ -4652,11 +4655,11 @@
       </c>
       <c r="N8" s="157">
         <f>+IF(I8&lt;&gt;0,K8/I8,0)</f>
-        <v>0.21280991735537191</v>
+        <v>0.21139705882352941</v>
       </c>
       <c r="O8" s="157">
         <f>+IF(J8&lt;&gt;0,K8/J8,0)</f>
-        <v>1.9433962264150944</v>
+        <v>1.7692307692307692</v>
       </c>
       <c r="P8" s="149">
         <f>SUMIF($B9:$B42,"&gt;0",P9:P42)</f>
@@ -4664,7 +4667,7 @@
       </c>
       <c r="Q8" s="149">
         <f>SUMIF($B9:$B42,"&gt;0",Q9:Q42)</f>
-        <v>26.5</v>
+        <v>32.5</v>
       </c>
       <c r="R8" s="155"/>
       <c r="S8" s="155"/>
@@ -4697,19 +4700,19 @@
       </c>
       <c r="I9" s="149">
         <f ca="1">SUMIF($B10:$B42,"&gt;0",I10:I15)</f>
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="J9" s="149">
         <f>SUMIF($B10:$B42,"&gt;0",J10:J42)</f>
-        <v>26.5</v>
+        <v>32.5</v>
       </c>
       <c r="K9" s="149">
         <f>SUMIF($B10:$B42,"&gt;0",K10:K42)</f>
-        <v>51.5</v>
+        <v>57.5</v>
       </c>
       <c r="L9" s="150">
         <f ca="1">+K9-I9</f>
-        <v>-190.5</v>
+        <v>-214.5</v>
       </c>
       <c r="M9" s="149">
         <f>+K9-J9</f>
@@ -4717,11 +4720,11 @@
       </c>
       <c r="N9" s="157">
         <f ca="1">+IF(I9&lt;&gt;0,K9/I9,0)</f>
-        <v>0.21280991735537191</v>
+        <v>0.21139705882352941</v>
       </c>
       <c r="O9" s="157">
         <f>+IF(J9&lt;&gt;0,K9/J9,0)</f>
-        <v>1.9433962264150944</v>
+        <v>1.7692307692307692</v>
       </c>
       <c r="P9" s="149">
         <f>SUMIF($B10:$B42,"&gt;0",P10:P42)</f>
@@ -4729,7 +4732,7 @@
       </c>
       <c r="Q9" s="149">
         <f>SUMIF($B10:$B42,"&gt;0",Q10:Q42)</f>
-        <v>26.5</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1">
@@ -5224,7 +5227,7 @@
       </c>
       <c r="Q17" s="151">
         <f>SUMIF($B18:$B22,"&gt;0",Q18:Q22)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1" outlineLevel="1">
@@ -5287,7 +5290,7 @@
       </c>
       <c r="Q18" s="153">
         <f>SUMIF($B19:$B22,"&gt;0",Q19:Q22)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:17" outlineLevel="2">
@@ -5381,15 +5384,15 @@
       </c>
       <c r="J20" s="151">
         <f>SUMIF($B21:$B35,"&gt;0",J21:J35)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K20" s="151">
         <f>SUMIF($B21:$B35,"&gt;0",K21:K35)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L20" s="152">
         <f>+K20-I20</f>
-        <v>-120</v>
+        <v>-114</v>
       </c>
       <c r="M20" s="151">
         <f>+K20-J20</f>
@@ -5397,11 +5400,11 @@
       </c>
       <c r="N20" s="158">
         <f>+IF(I20&lt;&gt;0,K20/I20,0)</f>
-        <v>1.6393442622950821E-2</v>
+        <v>6.5573770491803282E-2</v>
       </c>
       <c r="O20" s="158">
         <f>+IF(J20&lt;&gt;0,K20/J20,0)</f>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="P20" s="151">
         <f>SUMIF($B21:$B35,"&gt;0",P21:P35)</f>
@@ -5409,7 +5412,7 @@
       </c>
       <c r="Q20" s="151">
         <f>SUMIF($B21:$B35,"&gt;0",Q21:Q35)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="12" customHeight="1" outlineLevel="1">
@@ -5446,15 +5449,15 @@
       </c>
       <c r="J21" s="153">
         <f>SUMIF($B22:$B35,"&gt;0",J22:J35)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K21" s="153">
         <f>SUMIF($B22:$B35,"&gt;0",K22:K35)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L21" s="153">
         <f>+K21-I21</f>
-        <v>-60</v>
+        <v>-57</v>
       </c>
       <c r="M21" s="153">
         <f>+K21-J21</f>
@@ -5462,11 +5465,11 @@
       </c>
       <c r="N21" s="159">
         <f>+IF(I21&lt;&gt;0,K21/I21,0)</f>
-        <v>1.6393442622950821E-2</v>
+        <v>6.5573770491803282E-2</v>
       </c>
       <c r="O21" s="159">
         <f>+IF(J21&lt;&gt;0,K21/J21,0)</f>
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="P21" s="153">
         <f>SUMIF($B22:$B35,"&gt;0",P22:P35)</f>
@@ -5474,7 +5477,7 @@
       </c>
       <c r="Q21" s="153">
         <f>SUMIF($B22:$B35,"&gt;0",Q22:Q35)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:17" outlineLevel="2">
@@ -5652,7 +5655,9 @@
       <c r="E25" s="43">
         <v>40303</v>
       </c>
-      <c r="F25" s="43"/>
+      <c r="F25" s="43">
+        <v>40317</v>
+      </c>
       <c r="G25" s="43"/>
       <c r="H25" s="154">
         <v>3</v>
@@ -5662,21 +5667,21 @@
         <v>3</v>
       </c>
       <c r="J25" s="113"/>
-      <c r="K25" s="113" t="str">
+      <c r="K25" s="113">
         <f>+IF(AND(F25&lt;&gt;"",H25&lt;&gt;""),IF(F25&lt;=Parâmetros!$B$6,IF(G25="",H25/2,IF(G25&gt;Parâmetros!$B$6,H25/2,H25)),0),"")</f>
-        <v/>
-      </c>
-      <c r="L25" s="113" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="L25" s="113">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-1.5</v>
       </c>
       <c r="M25" s="113" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="N25" s="160" t="str">
+      <c r="N25" s="160">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="O25" s="172" t="str">
         <f t="shared" si="5"/>
@@ -5872,7 +5877,9 @@
       <c r="E29" s="43">
         <v>40304</v>
       </c>
-      <c r="F29" s="43"/>
+      <c r="F29" s="43">
+        <v>40317</v>
+      </c>
       <c r="G29" s="43"/>
       <c r="H29" s="154">
         <v>3</v>
@@ -5881,26 +5888,28 @@
         <f>+IF(AND(D29&lt;&gt;"",E29&lt;&gt;"",H29&lt;&gt;""),IF(D29&lt;Parâmetros!$B$6,IF(E29&gt;Parâmetros!$B$6,H29/2,H29),0),"")</f>
         <v>3</v>
       </c>
-      <c r="J29" s="113"/>
-      <c r="K29" s="113" t="str">
+      <c r="J29" s="113">
+        <v>3</v>
+      </c>
+      <c r="K29" s="113">
         <f>+IF(AND(F29&lt;&gt;"",H29&lt;&gt;""),IF(F29&lt;=Parâmetros!$B$6,IF(G29="",H29/2,IF(G29&gt;Parâmetros!$B$6,H29/2,H29)),0),"")</f>
-        <v/>
-      </c>
-      <c r="L29" s="113" t="str">
+        <v>1.5</v>
+      </c>
+      <c r="L29" s="113">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="M29" s="113" t="str">
+        <v>-1.5</v>
+      </c>
+      <c r="M29" s="113">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="N29" s="160" t="str">
+        <v>-1.5</v>
+      </c>
+      <c r="N29" s="160">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="O29" s="172" t="str">
+        <v>0.5</v>
+      </c>
+      <c r="O29" s="172">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0.5</v>
       </c>
       <c r="P29" s="113">
         <f t="shared" si="6"/>
@@ -5908,7 +5917,7 @@
       </c>
       <c r="Q29" s="113">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:17" outlineLevel="2">
@@ -6259,7 +6268,7 @@
       </c>
       <c r="I36" s="151">
         <f>SUMIF($B37:$B42,"&gt;0",I37:I42)</f>
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="J36" s="151">
         <f>SUMIF($B37:$B42,"&gt;0",J37:J42)</f>
@@ -6271,7 +6280,7 @@
       </c>
       <c r="L36" s="152">
         <f>+K36-I36</f>
-        <v>-57</v>
+        <v>-87</v>
       </c>
       <c r="M36" s="151">
         <f>+K36-J36</f>
@@ -6435,7 +6444,7 @@
       </c>
       <c r="I39" s="113">
         <f>+IF(AND(D39&lt;&gt;"",E39&lt;&gt;"",H39&lt;&gt;""),IF(D39&lt;Parâmetros!$B$6,IF(E39&gt;Parâmetros!$B$6,H39/2,H39),0),"")</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="J39" s="113"/>
       <c r="K39" s="113" t="str">
@@ -6490,7 +6499,7 @@
       </c>
       <c r="I40" s="113">
         <f>+IF(AND(D40&lt;&gt;"",E40&lt;&gt;"",H40&lt;&gt;""),IF(D40&lt;Parâmetros!$B$6,IF(E40&gt;Parâmetros!$B$6,H40/2,H40),0),"")</f>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="J40" s="113"/>
       <c r="K40" s="113" t="str">
@@ -6545,7 +6554,7 @@
       </c>
       <c r="I41" s="113">
         <f>+IF(AND(D41&lt;&gt;"",E41&lt;&gt;"",H41&lt;&gt;""),IF(D41&lt;Parâmetros!$B$6,IF(E41&gt;Parâmetros!$B$6,H41/2,H41),0),"")</f>
-        <v>13.5</v>
+        <v>27</v>
       </c>
       <c r="J41" s="113"/>
       <c r="K41" s="113" t="str">
@@ -6769,7 +6778,7 @@
     <mergeCell ref="P5:Q5"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31:C35 C21:C29 C38:C42 C19 C12:C16">
       <formula1>Recursos</formula1>
     </dataValidation>
@@ -6791,8 +6800,8 @@
   <sheetPr codeName="Plan6"/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -6825,7 +6834,7 @@
       <c r="D2" s="95"/>
       <c r="E2" s="95" t="str">
         <f>CONCATENATE("Data Base: ",TEXT(Parâmetros!$B$6,"dd/mm/aaaa"))</f>
-        <v>Data Base: 19/05/2010</v>
+        <v>Data Base: 21/05/2010</v>
       </c>
       <c r="F2" s="41"/>
       <c r="G2" s="100"/>
@@ -6876,7 +6885,9 @@
       <c r="C6" s="116" t="s">
         <v>216</v>
       </c>
-      <c r="D6" s="117"/>
+      <c r="D6" s="117" t="s">
+        <v>259</v>
+      </c>
       <c r="E6" s="119">
         <v>272</v>
       </c>
@@ -7007,7 +7018,7 @@
         <v>179</v>
       </c>
       <c r="B6" s="142">
-        <v>40317</v>
+        <v>40319</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>

<commit_message>
Finalização da implementação do A01 do UC11
</commit_message>
<xml_diff>
--- a/Gerência de Projetos/War - Acompanhamento de Projeto.xlsx
+++ b/Gerência de Projetos/War - Acompanhamento de Projeto.xlsx
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="260">
   <si>
     <t>Classificação Padrão de Produtos e Serviços</t>
   </si>
@@ -2326,6 +2326,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2337,9 +2359,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2365,25 +2384,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2584,11 +2584,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="59044224"/>
-        <c:axId val="59045760"/>
+        <c:axId val="51507584"/>
+        <c:axId val="51509120"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59044224"/>
+        <c:axId val="51507584"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2620,7 +2620,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59045760"/>
+        <c:crossAx val="51509120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2628,7 +2628,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59045760"/>
+        <c:axId val="51509120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2670,7 +2670,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59044224"/>
+        <c:crossAx val="51507584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -2716,7 +2716,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598500000387" footer="0.49212598500000387"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598500000393" footer="0.49212598500000393"/>
     <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2754,7 +2754,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.31531602468610342"/>
-          <c:y val="3.2418952618454226E-2"/>
+          <c:y val="3.2418952618454233E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -2771,9 +2771,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.11261286030066738"/>
-          <c:y val="0.14962593516209652"/>
-          <c:w val="0.65090233253786323"/>
-          <c:h val="0.73815461346633982"/>
+          <c:y val="0.14962593516209657"/>
+          <c:w val="0.65090233253786334"/>
+          <c:h val="0.73815461346633993"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2810,6 +2810,9 @@
                 <c:pt idx="2">
                   <c:v>40327</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>40329</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2826,6 +2829,9 @@
                   <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="#,##0">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
                   <c:v>272</c:v>
                 </c:pt>
               </c:numCache>
@@ -2864,6 +2870,9 @@
                 <c:pt idx="2">
                   <c:v>40327</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>40329</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2881,6 +2890,9 @@
                 </c:pt>
                 <c:pt idx="2" formatCode="#,##0">
                   <c:v>50.5</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>62.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2925,6 +2937,9 @@
                 <c:pt idx="2">
                   <c:v>40327</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>40329</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -2943,16 +2958,19 @@
                 <c:pt idx="2" formatCode="#,##0">
                   <c:v>85</c:v>
                 </c:pt>
+                <c:pt idx="3" formatCode="#,##0">
+                  <c:v>101.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="59189888"/>
-        <c:axId val="59212544"/>
+        <c:axId val="61811328"/>
+        <c:axId val="61833984"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="59189888"/>
+        <c:axId val="61811328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2984,7 +3002,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59212544"/>
+        <c:crossAx val="61833984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -2992,7 +3010,7 @@
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="59212544"/>
+        <c:axId val="61833984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -3035,7 +3053,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59189888"/>
+        <c:crossAx val="61811328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3058,9 +3076,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.7972972972972977"/>
-          <c:y val="0.46882793017456686"/>
+          <c:y val="0.46882793017456692"/>
           <c:w val="0.17792792792792791"/>
-          <c:h val="0.10972568578553772"/>
+          <c:h val="0.10972568578553775"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -3125,7 +3143,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598500000387" footer="0.49212598500000387"/>
+    <c:pageMargins b="0.98425196899999956" l="0.78740157499999996" r="0.78740157499999996" t="0.98425196899999956" header="0.49212598500000393" footer="0.49212598500000393"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3616,8 +3634,8 @@
   </sheetPr>
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51:J51"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3662,7 +3680,7 @@
       <c r="I2" s="163"/>
       <c r="J2" s="126">
         <f>Parâmetros!B6</f>
-        <v>40327</v>
+        <v>40329</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="6" customHeight="1" thickTop="1"/>
@@ -3673,16 +3691,16 @@
     </row>
     <row r="5" spans="1:11" ht="6" customHeight="1"/>
     <row r="6" spans="1:11" s="137" customFormat="1" ht="27" customHeight="1">
-      <c r="A6" s="201"/>
-      <c r="B6" s="202"/>
-      <c r="C6" s="202"/>
-      <c r="D6" s="202"/>
-      <c r="E6" s="202"/>
-      <c r="F6" s="202"/>
-      <c r="G6" s="202"/>
-      <c r="H6" s="202"/>
-      <c r="I6" s="202"/>
-      <c r="J6" s="202"/>
+      <c r="A6" s="184"/>
+      <c r="B6" s="185"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
+      <c r="I6" s="185"/>
+      <c r="J6" s="185"/>
       <c r="K6" s="136"/>
     </row>
     <row r="7" spans="1:11" s="137" customFormat="1" ht="6" customHeight="1">
@@ -3720,7 +3738,7 @@
       <c r="B11" s="74"/>
       <c r="C11" s="118">
         <f>IF(Planejamento!H8&lt;&gt;0,VLOOKUP(Parâmetros!B6,A49:I139,4)/Planejamento!H8,0)</f>
-        <v>0.3125</v>
+        <v>0.37316176470588236</v>
       </c>
       <c r="F11" s="99"/>
       <c r="G11" s="100"/>
@@ -3849,7 +3867,7 @@
       <c r="B22" s="105"/>
       <c r="C22" s="92">
         <f>Planejamento!J8</f>
-        <v>50.5</v>
+        <v>62.5</v>
       </c>
       <c r="K22" s="98"/>
     </row>
@@ -3860,7 +3878,7 @@
       <c r="B23" s="105"/>
       <c r="C23" s="92">
         <f>VLOOKUP(Parâmetros!B6,A49:I136,9)</f>
-        <v>161.60000000000002</v>
+        <v>167.48768472906403</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -3895,17 +3913,17 @@
       <c r="K25" s="90"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="190" t="s">
+      <c r="A26" s="197" t="s">
         <v>210</v>
       </c>
-      <c r="B26" s="188" t="s">
+      <c r="B26" s="196" t="s">
         <v>207</v>
       </c>
-      <c r="C26" s="189"/>
-      <c r="D26" s="188" t="s">
+      <c r="C26" s="188"/>
+      <c r="D26" s="196" t="s">
         <v>211</v>
       </c>
-      <c r="E26" s="189"/>
+      <c r="E26" s="188"/>
       <c r="F26" s="89"/>
       <c r="G26" s="93"/>
       <c r="H26" s="93"/>
@@ -3914,7 +3932,7 @@
       <c r="K26" s="90"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="191"/>
+      <c r="A27" s="198"/>
       <c r="B27" s="164" t="s">
         <v>230</v>
       </c>
@@ -4040,27 +4058,27 @@
     </row>
     <row r="41" spans="1:11" ht="12.75" customHeight="1">
       <c r="A41" s="72"/>
-      <c r="B41" s="199" t="s">
+      <c r="B41" s="206" t="s">
         <v>223</v>
       </c>
-      <c r="C41" s="203" t="s">
+      <c r="C41" s="186" t="s">
         <v>151</v>
       </c>
-      <c r="D41" s="204"/>
-      <c r="E41" s="204"/>
-      <c r="F41" s="189"/>
-      <c r="G41" s="205" t="s">
+      <c r="D41" s="187"/>
+      <c r="E41" s="187"/>
+      <c r="F41" s="188"/>
+      <c r="G41" s="189" t="s">
         <v>160</v>
       </c>
-      <c r="H41" s="206"/>
-      <c r="I41" s="206"/>
-      <c r="J41" s="207"/>
+      <c r="H41" s="190"/>
+      <c r="I41" s="190"/>
+      <c r="J41" s="191"/>
     </row>
     <row r="42" spans="1:11" ht="24.75" customHeight="1">
       <c r="A42" s="85" t="s">
         <v>169</v>
       </c>
-      <c r="B42" s="200"/>
+      <c r="B42" s="207"/>
       <c r="C42" s="86" t="s">
         <v>187</v>
       </c>
@@ -4121,11 +4139,11 @@
       </c>
       <c r="I43" s="173">
         <f>Planejamento!J9</f>
-        <v>50.5</v>
+        <v>62.5</v>
       </c>
       <c r="J43" s="173">
         <f>Planejamento!K9</f>
-        <v>85</v>
+        <v>101.5</v>
       </c>
       <c r="K43" s="107">
         <f>+D43-C43</f>
@@ -4166,19 +4184,19 @@
       <c r="A47" s="83"/>
       <c r="B47" s="83"/>
       <c r="C47" s="83"/>
-      <c r="D47" s="186" t="s">
+      <c r="D47" s="194" t="s">
         <v>189</v>
       </c>
-      <c r="E47" s="196" t="s">
+      <c r="E47" s="203" t="s">
         <v>159</v>
       </c>
-      <c r="F47" s="197"/>
-      <c r="G47" s="197"/>
-      <c r="H47" s="198"/>
-      <c r="I47" s="192" t="s">
+      <c r="F47" s="204"/>
+      <c r="G47" s="204"/>
+      <c r="H47" s="205"/>
+      <c r="I47" s="199" t="s">
         <v>184</v>
       </c>
-      <c r="J47" s="193"/>
+      <c r="J47" s="200"/>
     </row>
     <row r="48" spans="1:11" ht="24.75" customHeight="1">
       <c r="A48" s="84" t="s">
@@ -4190,7 +4208,7 @@
       <c r="C48" s="103" t="s">
         <v>154</v>
       </c>
-      <c r="D48" s="187"/>
+      <c r="D48" s="195"/>
       <c r="E48" s="69" t="s">
         <v>155</v>
       </c>
@@ -4203,8 +4221,8 @@
       <c r="H48" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="I48" s="194"/>
-      <c r="J48" s="195"/>
+      <c r="I48" s="201"/>
+      <c r="J48" s="202"/>
     </row>
     <row r="49" spans="1:10" ht="12">
       <c r="A49" s="142">
@@ -4235,11 +4253,11 @@
         <f t="shared" ref="H49" si="5">+IF(C49&lt;&gt;0,D49/C49,0)</f>
         <v>1.9285714285714286</v>
       </c>
-      <c r="I49" s="184">
+      <c r="I49" s="192">
         <f>IF(H49&lt;&gt;0,C49+(VLOOKUP(A49,'Histórico de Versões'!A5:E72,5)-D49)/H49,"")</f>
         <v>141.03703703703704</v>
       </c>
-      <c r="J49" s="185"/>
+      <c r="J49" s="193"/>
     </row>
     <row r="50" spans="1:10" ht="12">
       <c r="A50" s="142">
@@ -4270,11 +4288,11 @@
         <f t="shared" ref="H50:H55" si="7">+IF(C50&lt;&gt;0,D50/C50,0)</f>
         <v>1.9433962264150944</v>
       </c>
-      <c r="I50" s="184">
+      <c r="I50" s="192">
         <f>IF(H50&lt;&gt;0,C50+(VLOOKUP(A50,'Histórico de Versões'!A6:E73,5)-D50)/H50,"")</f>
         <v>139.96116504854371</v>
       </c>
-      <c r="J50" s="185"/>
+      <c r="J50" s="193"/>
     </row>
     <row r="51" spans="1:10" ht="12">
       <c r="A51" s="142">
@@ -4305,38 +4323,46 @@
         <f t="shared" si="7"/>
         <v>1.6831683168316831</v>
       </c>
-      <c r="I51" s="184">
+      <c r="I51" s="192">
         <f>IF(H51&lt;&gt;0,C51+(VLOOKUP(A51,'Histórico de Versões'!A7:E74,5)-D51)/H51,"")</f>
         <v>161.60000000000002</v>
       </c>
-      <c r="J51" s="185"/>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="106"/>
-      <c r="B52" s="129"/>
-      <c r="C52" s="129"/>
-      <c r="D52" s="129"/>
+      <c r="J51" s="193"/>
+    </row>
+    <row r="52" spans="1:10" ht="12">
+      <c r="A52" s="142">
+        <v>40329</v>
+      </c>
+      <c r="B52" s="129">
+        <v>272</v>
+      </c>
+      <c r="C52" s="129">
+        <v>62.5</v>
+      </c>
+      <c r="D52" s="129">
+        <v>101.5</v>
+      </c>
       <c r="E52" s="113">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-170.5</v>
       </c>
       <c r="F52" s="113">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="G52" s="65">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.37316176470588236</v>
       </c>
       <c r="H52" s="65">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="I52" s="184" t="str">
+        <v>1.6240000000000001</v>
+      </c>
+      <c r="I52" s="192">
         <f>IF(H52&lt;&gt;0,C52+(VLOOKUP(A52,'Histórico de Versões'!A8:E75,5)-D52)/H52,"")</f>
-        <v/>
-      </c>
-      <c r="J52" s="185"/>
+        <v>167.48768472906403</v>
+      </c>
+      <c r="J52" s="193"/>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="106"/>
@@ -4359,11 +4385,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I53" s="184" t="str">
+      <c r="I53" s="192" t="str">
         <f>IF(H53&lt;&gt;0,C53+(VLOOKUP(A53,'Histórico de Versões'!A9:E76,5)-D53)/H53,"")</f>
         <v/>
       </c>
-      <c r="J53" s="185"/>
+      <c r="J53" s="193"/>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="106"/>
@@ -4386,11 +4412,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I54" s="184" t="str">
+      <c r="I54" s="192" t="str">
         <f>IF(H54&lt;&gt;0,C54+(VLOOKUP(A54,'Histórico de Versões'!A10:E77,5)-D54)/H54,"")</f>
         <v/>
       </c>
-      <c r="J54" s="185"/>
+      <c r="J54" s="193"/>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="106"/>
@@ -4413,11 +4439,11 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I55" s="184" t="str">
+      <c r="I55" s="192" t="str">
         <f>IF(H55&lt;&gt;0,C55+(VLOOKUP(A55,'Histórico de Versões'!A11:E78,5)-D55)/H55,"")</f>
         <v/>
       </c>
-      <c r="J55" s="185"/>
+      <c r="J55" s="193"/>
     </row>
     <row r="56" spans="1:10">
       <c r="B56" s="90"/>
@@ -4432,6 +4458,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="I54:J54"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="C41:F41"/>
     <mergeCell ref="G41:J41"/>
@@ -4448,7 +4475,6 @@
     <mergeCell ref="I51:J51"/>
     <mergeCell ref="I52:J52"/>
     <mergeCell ref="I53:J53"/>
-    <mergeCell ref="I54:J54"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.59055118110236227" right="0.51181102362204722" top="0.59055118110236227" bottom="0.59055118110236227" header="0.51181102362204722" footer="0.51181102362204722"/>
@@ -4469,7 +4495,7 @@
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A137" sqref="A137"/>
-      <selection pane="topRight" activeCell="H8" sqref="H8"/>
+      <selection pane="topRight" activeCell="I8" sqref="I8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="2"/>
@@ -4532,7 +4558,7 @@
       <c r="S2" s="146"/>
       <c r="T2" s="95" t="str">
         <f>CONCATENATE("Data Base: ",TEXT(Parâmetros!$B$6,"dd/mm/aaaa"))</f>
-        <v>Data Base: 29/05/2010</v>
+        <v>Data Base: 31/05/2010</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="20.25" customHeight="1" thickTop="1">
@@ -4543,7 +4569,7 @@
       <c r="A5" s="72"/>
       <c r="B5" s="170"/>
       <c r="C5" s="178"/>
-      <c r="D5" s="203" t="s">
+      <c r="D5" s="186" t="s">
         <v>151</v>
       </c>
       <c r="E5" s="208"/>
@@ -4554,7 +4580,7 @@
       </c>
       <c r="I5" s="211"/>
       <c r="J5" s="212"/>
-      <c r="K5" s="196" t="s">
+      <c r="K5" s="203" t="s">
         <v>159</v>
       </c>
       <c r="L5" s="213"/>
@@ -4665,27 +4691,27 @@
       </c>
       <c r="J8" s="149">
         <f>SUMIF($B9:$B42,"&gt;0",J9:J42)</f>
-        <v>50.5</v>
+        <v>62.5</v>
       </c>
       <c r="K8" s="149">
         <f>SUMIF($B9:$B42,"&gt;0",K9:K42)</f>
-        <v>85</v>
+        <v>101.5</v>
       </c>
       <c r="L8" s="150">
         <f>+K8-I8</f>
-        <v>-187</v>
+        <v>-170.5</v>
       </c>
       <c r="M8" s="149">
         <f>+K8-J8</f>
-        <v>34.5</v>
+        <v>39</v>
       </c>
       <c r="N8" s="157">
         <f>+IF(I8&lt;&gt;0,K8/I8,0)</f>
-        <v>0.3125</v>
+        <v>0.37316176470588236</v>
       </c>
       <c r="O8" s="157">
         <f>+IF(J8&lt;&gt;0,K8/J8,0)</f>
-        <v>1.6831683168316831</v>
+        <v>1.6240000000000001</v>
       </c>
       <c r="P8" s="149">
         <f>SUMIF($B9:$B42,"&gt;0",P9:P42)</f>
@@ -4693,7 +4719,7 @@
       </c>
       <c r="Q8" s="149">
         <f>SUMIF($B9:$B42,"&gt;0",Q9:Q42)</f>
-        <v>50.5</v>
+        <v>62.5</v>
       </c>
       <c r="R8" s="155"/>
       <c r="S8" s="155"/>
@@ -4730,27 +4756,27 @@
       </c>
       <c r="J9" s="149">
         <f>SUMIF($B10:$B42,"&gt;0",J10:J42)</f>
-        <v>50.5</v>
+        <v>62.5</v>
       </c>
       <c r="K9" s="149">
         <f>SUMIF($B10:$B42,"&gt;0",K10:K42)</f>
-        <v>85</v>
+        <v>101.5</v>
       </c>
       <c r="L9" s="150">
         <f ca="1">+K9-I9</f>
-        <v>-187</v>
+        <v>-170.5</v>
       </c>
       <c r="M9" s="149">
         <f>+K9-J9</f>
-        <v>34.5</v>
+        <v>39</v>
       </c>
       <c r="N9" s="157">
         <f ca="1">+IF(I9&lt;&gt;0,K9/I9,0)</f>
-        <v>0.3125</v>
+        <v>0.37316176470588236</v>
       </c>
       <c r="O9" s="157">
         <f>+IF(J9&lt;&gt;0,K9/J9,0)</f>
-        <v>1.6831683168316831</v>
+        <v>1.6240000000000001</v>
       </c>
       <c r="P9" s="149">
         <f>SUMIF($B10:$B42,"&gt;0",P10:P42)</f>
@@ -4758,7 +4784,7 @@
       </c>
       <c r="Q9" s="149">
         <f>SUMIF($B10:$B42,"&gt;0",Q10:Q42)</f>
-        <v>50.5</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1">
@@ -5253,7 +5279,7 @@
       </c>
       <c r="Q17" s="151">
         <f>SUMIF($B18:$B22,"&gt;0",Q18:Q22)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="12" customHeight="1" outlineLevel="1">
@@ -5316,7 +5342,7 @@
       </c>
       <c r="Q18" s="153">
         <f>SUMIF($B19:$B22,"&gt;0",Q19:Q22)</f>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:17" outlineLevel="2">
@@ -5410,27 +5436,27 @@
       </c>
       <c r="J20" s="151">
         <f>SUMIF($B21:$B35,"&gt;0",J21:J35)</f>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="K20" s="151">
         <f>SUMIF($B21:$B35,"&gt;0",K21:K35)</f>
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="L20" s="152">
         <f>+K20-I20</f>
-        <v>-94</v>
+        <v>-85</v>
       </c>
       <c r="M20" s="151">
         <f>+K20-J20</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N20" s="158">
         <f>+IF(I20&lt;&gt;0,K20/I20,0)</f>
-        <v>0.22950819672131148</v>
+        <v>0.30327868852459017</v>
       </c>
       <c r="O20" s="158">
         <f>+IF(J20&lt;&gt;0,K20/J20,0)</f>
-        <v>1.2727272727272727</v>
+        <v>1.2333333333333334</v>
       </c>
       <c r="P20" s="151">
         <f>SUMIF($B21:$B35,"&gt;0",P21:P35)</f>
@@ -5438,7 +5464,7 @@
       </c>
       <c r="Q20" s="151">
         <f>SUMIF($B21:$B35,"&gt;0",Q21:Q35)</f>
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="12" customHeight="1" outlineLevel="1">
@@ -5475,27 +5501,27 @@
       </c>
       <c r="J21" s="153">
         <f>SUMIF($B22:$B35,"&gt;0",J22:J35)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K21" s="153">
         <f>SUMIF($B22:$B35,"&gt;0",K22:K35)</f>
-        <v>14</v>
+        <v>18.5</v>
       </c>
       <c r="L21" s="153">
         <f>+K21-I21</f>
-        <v>-47</v>
+        <v>-42.5</v>
       </c>
       <c r="M21" s="153">
         <f>+K21-J21</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="N21" s="159">
         <f>+IF(I21&lt;&gt;0,K21/I21,0)</f>
-        <v>0.22950819672131148</v>
+        <v>0.30327868852459017</v>
       </c>
       <c r="O21" s="159">
         <f>+IF(J21&lt;&gt;0,K21/J21,0)</f>
-        <v>1.2727272727272727</v>
+        <v>1.2333333333333334</v>
       </c>
       <c r="P21" s="153">
         <f>SUMIF($B22:$B35,"&gt;0",P22:P35)</f>
@@ -5503,7 +5529,7 @@
       </c>
       <c r="Q21" s="153">
         <f>SUMIF($B22:$B35,"&gt;0",Q22:Q35)</f>
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:17" outlineLevel="2">
@@ -5908,7 +5934,9 @@
       <c r="F29" s="43">
         <v>40317</v>
       </c>
-      <c r="G29" s="43"/>
+      <c r="G29" s="43">
+        <v>40329</v>
+      </c>
       <c r="H29" s="154">
         <v>3</v>
       </c>
@@ -5917,27 +5945,27 @@
         <v>3</v>
       </c>
       <c r="J29" s="113">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K29" s="113">
         <f>+IF(AND(F29&lt;&gt;"",H29&lt;&gt;""),IF(F29&lt;=Parâmetros!$B$6,IF(G29="",H29/2,IF(G29&gt;Parâmetros!$B$6,H29/2,H29)),0),"")</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="L29" s="113">
         <f t="shared" si="2"/>
-        <v>-1.5</v>
+        <v>0</v>
       </c>
       <c r="M29" s="113">
         <f t="shared" si="3"/>
-        <v>-4.5</v>
+        <v>-5</v>
       </c>
       <c r="N29" s="160">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O29" s="172">
         <f t="shared" si="5"/>
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="P29" s="113">
         <f t="shared" si="6"/>
@@ -5945,7 +5973,7 @@
       </c>
       <c r="Q29" s="113">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:17" outlineLevel="2">
@@ -6232,7 +6260,9 @@
       <c r="F35" s="43">
         <v>40317</v>
       </c>
-      <c r="G35" s="43"/>
+      <c r="G35" s="43">
+        <v>40329</v>
+      </c>
       <c r="H35" s="154">
         <v>6</v>
       </c>
@@ -6241,27 +6271,27 @@
         <v>6</v>
       </c>
       <c r="J35" s="113">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K35" s="113">
         <f>+IF(AND(F35&lt;&gt;"",H35&lt;&gt;""),IF(F35&lt;=Parâmetros!$B$6,IF(G35="",H35/2,IF(G35&gt;Parâmetros!$B$6,H35/2,H35)),0),"")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L35" s="113">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="M35" s="113">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="160">
         <f t="shared" si="4"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O35" s="172">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="P35" s="113">
         <f t="shared" si="6"/>
@@ -6269,7 +6299,7 @@
       </c>
       <c r="Q35" s="113">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="15" customHeight="1">
@@ -6304,27 +6334,27 @@
       </c>
       <c r="J36" s="151">
         <f>SUMIF($B37:$B42,"&gt;0",J37:J42)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K36" s="151">
         <f>SUMIF($B37:$B42,"&gt;0",K37:K42)</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="L36" s="152">
         <f>+K36-I36</f>
-        <v>-79.5</v>
+        <v>-72</v>
       </c>
       <c r="M36" s="151">
         <f>+K36-J36</f>
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="N36" s="158">
         <f>+IF(I36&lt;&gt;0,K36/I36,0)</f>
-        <v>8.6206896551724144E-2</v>
+        <v>0.17241379310344829</v>
       </c>
       <c r="O36" s="158">
         <f>+IF(J36&lt;&gt;0,K36/J36,0)</f>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="P36" s="151" t="e">
         <f>SUMIF(#REF!,"&gt;0",P37:P38)</f>
@@ -6332,7 +6362,7 @@
       </c>
       <c r="Q36" s="151">
         <f>SUMIF($B37:$B42,"&gt;0",Q37:Q42)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="22.5" outlineLevel="1">
@@ -6367,19 +6397,19 @@
       </c>
       <c r="J37" s="153">
         <f>SUMIF($B38:$B42,"&gt;0",J38:J42)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K37" s="153">
         <f>SUMIF($B38:$B42,"&gt;0",K38:K42)</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="L37" s="153">
         <f>+K37-I37</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="M37" s="153">
         <f>+K37-J37</f>
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="N37" s="159">
         <f>+IF(I37&lt;&gt;0,K37/I37,0)</f>
@@ -6387,7 +6417,7 @@
       </c>
       <c r="O37" s="159">
         <f>+IF(J37&lt;&gt;0,K37/J37,0)</f>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="P37" s="153">
         <f>SUMIF($B38:$B42,"&gt;0",P38:P42)</f>
@@ -6395,7 +6425,7 @@
       </c>
       <c r="Q37" s="153">
         <f>SUMIF($B38:$B42,"&gt;0",Q38:Q42)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:17" outlineLevel="2">
@@ -6637,7 +6667,9 @@
       <c r="F42" s="43">
         <v>40326</v>
       </c>
-      <c r="G42" s="43"/>
+      <c r="G42" s="43">
+        <v>40329</v>
+      </c>
       <c r="H42" s="154">
         <v>15</v>
       </c>
@@ -6646,27 +6678,27 @@
         <v>15</v>
       </c>
       <c r="J42" s="113">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K42" s="113">
         <f>+IF(AND(F42&lt;&gt;"",H42&lt;&gt;""),IF(F42&lt;=Parâmetros!$B$6,IF(G42="",H42/2,IF(G42&gt;Parâmetros!$B$6,H42/2,H42)),0),"")</f>
-        <v>7.5</v>
+        <v>15</v>
       </c>
       <c r="L42" s="113">
         <f>IF(AND(A42&gt;0,K42&lt;&gt;"",I42&lt;&gt;""),+K42-I42,"")</f>
-        <v>-7.5</v>
+        <v>0</v>
       </c>
       <c r="M42" s="113">
         <f>IF(AND(A42&gt;0,K42&lt;&gt;"",J42&lt;&gt;""),K42-J42,"")</f>
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="N42" s="160">
         <f>+IF(AND(A42&gt;0,I42&lt;&gt;0,I42&lt;&gt;"",K42&lt;&gt;""),K42/I42,"")</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="O42" s="172">
         <f>+IF(AND(A42&gt;0,K42&lt;&gt;"",J42&lt;&gt;0,J42&lt;&gt;""),K42/J42,"")</f>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="P42" s="113">
         <f t="shared" si="8"/>
@@ -6674,7 +6706,7 @@
       </c>
       <c r="Q42" s="113">
         <f t="shared" si="9"/>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:17">
@@ -6837,7 +6869,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -6870,7 +6902,7 @@
       <c r="D2" s="95"/>
       <c r="E2" s="95" t="str">
         <f>CONCATENATE("Data Base: ",TEXT(Parâmetros!$B$6,"dd/mm/aaaa"))</f>
-        <v>Data Base: 29/05/2010</v>
+        <v>Data Base: 31/05/2010</v>
       </c>
       <c r="F2" s="41"/>
       <c r="G2" s="100"/>
@@ -6944,11 +6976,19 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="10.5" customHeight="1">
-      <c r="A8" s="142"/>
+      <c r="A8" s="142">
+        <v>40329</v>
+      </c>
       <c r="B8" s="116"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="117"/>
-      <c r="E8" s="119"/>
+      <c r="C8" s="116" t="s">
+        <v>216</v>
+      </c>
+      <c r="D8" s="117" t="s">
+        <v>259</v>
+      </c>
+      <c r="E8" s="119">
+        <v>272</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="10.5" customHeight="1">
       <c r="A9" s="142"/>
@@ -7062,7 +7102,7 @@
         <v>179</v>
       </c>
       <c r="B6" s="142">
-        <v>40327</v>
+        <v>40329</v>
       </c>
     </row>
     <row r="8" spans="1:6">

</xml_diff>